<commit_message>
update commit on realestate project
</commit_message>
<xml_diff>
--- a/property/property.xlsx
+++ b/property/property.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>broker</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>photos/istockphoto-479842074-612x612.jpg</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>India</t>
   </si>
 </sst>
 </file>
@@ -459,15 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,46 +484,49 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -528,42 +537,45 @@
         <v>21</v>
       </c>
       <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>20000000</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
       </c>
       <c r="J2">
         <v>4</v>
       </c>
       <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
         <v>0</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>2090</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>25</v>
       </c>
-      <c r="P2" t="b">
+      <c r="Q2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>